<commit_message>
OP Codes in excel sheet
</commit_message>
<xml_diff>
--- a/Docs/opCode.xlsx
+++ b/Docs/opCode.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP\CMP5\Arch\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP\CMP5\Arch\project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED57B9C3-FDF2-41C9-9E98-BBFC63910375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A38311B-E13D-41F4-B139-12566D6DABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>00_001_000</t>
   </si>
@@ -172,18 +172,6 @@
     <t>RTI</t>
   </si>
   <si>
-    <t>11_110_010</t>
-  </si>
-  <si>
-    <t>INTR</t>
-  </si>
-  <si>
-    <t>11_011_000</t>
-  </si>
-  <si>
-    <t>RESET</t>
-  </si>
-  <si>
     <t>10_111_000</t>
   </si>
   <si>
@@ -194,13 +182,100 @@
   </si>
   <si>
     <t>01_000_101</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>2 operands src &amp; dst</t>
+  </si>
+  <si>
+    <t>2 operands dst &amp; immediate</t>
+  </si>
+  <si>
+    <t>1 operand dst</t>
+  </si>
+  <si>
+    <t>zero operands</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>ALU operation</t>
+  </si>
+  <si>
+    <t>STORE</t>
+  </si>
+  <si>
+    <t>LOAD</t>
+  </si>
+  <si>
+    <t>JMP (Changes PC only)</t>
+  </si>
+  <si>
+    <t>something else</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>Changes PC and Stack</t>
+  </si>
+  <si>
+    <t>Changes Stack</t>
+  </si>
+  <si>
+    <t>B15:B14</t>
+  </si>
+  <si>
+    <t>B13:B11</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>B15:B8</t>
+  </si>
+  <si>
+    <t>Instruction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -210,6 +285,11 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -234,9 +314,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,251 +538,368 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" style="3"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>

</xml_diff>